<commit_message>
reading the body section for all wells
</commit_message>
<xml_diff>
--- a/src/main/resources/static/mergedCells.xlsx
+++ b/src/main/resources/static/mergedCells.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\upwork tasks\history-Migration\src\main\resources\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programming-projects\jwt\JWTdemo\History_Migration\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
   <si>
     <t>WELL ( S/R ) :    A-72</t>
   </si>
@@ -1380,77 +1380,77 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1738,9 +1738,9 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C163" sqref="C163:J163"/>
-      <selection pane="bottomLeft" activeCell="B36" sqref="B36:B40"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1808,8 +1808,8 @@
       <c r="D3" s="60"/>
       <c r="E3" s="60"/>
       <c r="F3" s="61"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="71"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="69"/>
       <c r="I3" s="64" t="s">
         <v>6</v>
       </c>
@@ -1844,26 +1844,26 @@
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="74" t="s">
+      <c r="B5" s="71"/>
+      <c r="C5" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="71"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="69"/>
       <c r="I5" s="64" t="s">
         <v>14</v>
       </c>
       <c r="J5" s="65"/>
-      <c r="K5" s="77" t="s">
+      <c r="K5" s="75" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="78"/>
+      <c r="L5" s="76"/>
       <c r="M5" s="3"/>
     </row>
     <row r="6" spans="1:13" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1911,16 +1911,16 @@
       <c r="B7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
       <c r="K7" s="12" t="s">
         <v>30</v>
       </c>
@@ -2011,7 +2011,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="79">
+      <c r="A11" s="77">
         <v>43637</v>
       </c>
       <c r="B11" s="21" t="s">
@@ -2031,7 +2031,7 @@
       <c r="L11" s="26"/>
     </row>
     <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="80"/>
+      <c r="A12" s="78"/>
       <c r="B12" s="21" t="s">
         <v>32</v>
       </c>
@@ -2253,16 +2253,16 @@
       <c r="B20" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="81" t="s">
+      <c r="C20" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
-      <c r="G20" s="82"/>
-      <c r="H20" s="82"/>
-      <c r="I20" s="82"/>
-      <c r="J20" s="83"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="81"/>
       <c r="K20" s="37"/>
       <c r="L20" s="38"/>
     </row>
@@ -2319,16 +2319,16 @@
       <c r="B23" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="84" t="s">
+      <c r="C23" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="85"/>
-      <c r="E23" s="85"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="85"/>
-      <c r="H23" s="85"/>
-      <c r="I23" s="85"/>
-      <c r="J23" s="86"/>
+      <c r="D23" s="83"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="83"/>
+      <c r="G23" s="83"/>
+      <c r="H23" s="83"/>
+      <c r="I23" s="83"/>
+      <c r="J23" s="84"/>
       <c r="K23" s="45"/>
       <c r="L23" s="46" t="s">
         <v>46</v>
@@ -2361,38 +2361,38 @@
       <c r="B25" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="84" t="s">
+      <c r="C25" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="85"/>
-      <c r="E25" s="85"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="85"/>
-      <c r="I25" s="85"/>
-      <c r="J25" s="86"/>
+      <c r="D25" s="83"/>
+      <c r="E25" s="83"/>
+      <c r="F25" s="83"/>
+      <c r="G25" s="83"/>
+      <c r="H25" s="83"/>
+      <c r="I25" s="83"/>
+      <c r="J25" s="84"/>
       <c r="K25" s="45"/>
       <c r="L25" s="46" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="79">
+      <c r="A26" s="77">
         <v>44016</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="87" t="s">
+      <c r="C26" s="85" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="89"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="86"/>
+      <c r="I26" s="86"/>
+      <c r="J26" s="87"/>
       <c r="K26" s="47" t="s">
         <v>51</v>
       </c>
@@ -2401,20 +2401,20 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="80"/>
+      <c r="A27" s="78"/>
       <c r="B27" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="84" t="s">
+      <c r="C27" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="90"/>
-      <c r="E27" s="90"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="90"/>
-      <c r="J27" s="91"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="88"/>
+      <c r="H27" s="88"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="89"/>
       <c r="K27" s="49"/>
       <c r="L27" s="46" t="s">
         <v>54</v>
@@ -2499,14 +2499,8 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
-      <c r="B32" s="50" t="s">
-        <v>55</v>
-      </c>
       <c r="C32" s="22"/>
-      <c r="D32" s="23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="D32" s="23"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
@@ -2619,7 +2613,7 @@
   </sheetData>
   <autoFilter ref="B6:K6"/>
   <mergeCells count="31">
-    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C7:J7"/>
     <mergeCell ref="C28:J28"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="C11:J11"/>
@@ -2629,21 +2623,21 @@
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="C26:J26"/>
     <mergeCell ref="C27:J27"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:F2"/>

</xml_diff>